<commit_message>
A3_jonathan oprettet. Premerge med endelig version hvor små fejl akkumulerer i bunden
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/IOdata_main_catalog.xlsx
+++ b/examples/Abatement/Data/IOdata_main_catalog.xlsx
@@ -47,18 +47,6 @@
     <t>qD/qD</t>
   </si>
   <si>
-    <t>basetech_EL_electricity</t>
-  </si>
-  <si>
-    <t>basetech_EL_oil</t>
-  </si>
-  <si>
-    <t>basetech_EL_K</t>
-  </si>
-  <si>
-    <t>basetech_EL_gas</t>
-  </si>
-  <si>
     <t>gas</t>
   </si>
   <si>
@@ -66,6 +54,18 @@
   </si>
   <si>
     <t>out1</t>
+  </si>
+  <si>
+    <t>basetech_EH_electricity</t>
+  </si>
+  <si>
+    <t>basetech_EH_oil</t>
+  </si>
+  <si>
+    <t>basetech_EH_gas</t>
+  </si>
+  <si>
+    <t>basetech_EH_K</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,13 +413,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>165</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -427,15 +427,15 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -443,36 +443,36 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>11</v>
@@ -480,10 +480,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lower bounds på currapp. Kan skrue IO i alm. calibrate. Kan skrue currapp i kataloger med middel omk
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/IOdata_main_catalog.xlsx
+++ b/examples/Abatement/Data/IOdata_main_catalog.xlsx
@@ -383,7 +383,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,13 +419,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -442,7 +442,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -459,7 +459,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -476,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -485,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="G5">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -493,7 +493,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A4 for jonathan. Samlet script til figurer.
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/IOdata_main_catalog.xlsx
+++ b/examples/Abatement/Data/IOdata_main_catalog.xlsx
@@ -434,7 +434,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -459,7 +459,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -468,7 +468,7 @@
         <v>7</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -476,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -485,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="G5">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Endogen elektricitetspris fungerer. Arbejder på figurerne til det
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/IOdata_main_catalog.xlsx
+++ b/examples/Abatement/Data/IOdata_main_catalog.xlsx
@@ -383,7 +383,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +419,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -434,7 +434,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>